<commit_message>
issue with vsync, gpu not being maximised
</commit_message>
<xml_diff>
--- a/PolygonsTest.xlsx
+++ b/PolygonsTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohhja\Documents\Github\Project\OpenGL\OpenGL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1A76D-5050-4955-A2E2-AB50D5A79B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F592A3-1AA8-49A6-82F9-09CC784D61B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="11">
   <si>
     <t>684 Polygons</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Laptop Turbo mode 684 polygons</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>19404 Polygons</t>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>2872804 Polygons</t>
+  </si>
+  <si>
+    <t>ALL WRONG, RTX GPU WAS NOT BEING USED AND NOT BEING MAXED OUT</t>
   </si>
 </sst>
 </file>
@@ -3619,20 +3619,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q90"/>
+  <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3640,90 +3640,255 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2586</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2329</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>2371</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <v>2261</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>2702</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>2682</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>2932</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>3633</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>1904</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>1556</v>
+      </c>
+      <c r="O12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
+      <c r="O19" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -3732,6 +3897,15 @@
       <c r="B20" t="s">
         <v>2</v>
       </c>
+      <c r="O20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P20" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -3740,6 +3914,15 @@
       <c r="B21">
         <v>3740</v>
       </c>
+      <c r="O21" t="s">
+        <v>10</v>
+      </c>
+      <c r="P21" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -3748,6 +3931,15 @@
       <c r="B22">
         <v>3511</v>
       </c>
+      <c r="O22" t="s">
+        <v>10</v>
+      </c>
+      <c r="P22" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -3756,6 +3948,15 @@
       <c r="B23">
         <v>3396</v>
       </c>
+      <c r="O23" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -3764,6 +3965,15 @@
       <c r="B24">
         <v>3688</v>
       </c>
+      <c r="O24" t="s">
+        <v>10</v>
+      </c>
+      <c r="P24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -3772,6 +3982,15 @@
       <c r="B25">
         <v>4314</v>
       </c>
+      <c r="O25" t="s">
+        <v>10</v>
+      </c>
+      <c r="P25" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -3780,6 +3999,15 @@
       <c r="B26">
         <v>4321</v>
       </c>
+      <c r="O26" t="s">
+        <v>10</v>
+      </c>
+      <c r="P26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -3788,6 +4016,15 @@
       <c r="B27">
         <v>4344</v>
       </c>
+      <c r="O27" t="s">
+        <v>10</v>
+      </c>
+      <c r="P27" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -3796,6 +4033,15 @@
       <c r="B28">
         <v>4017</v>
       </c>
+      <c r="O28" t="s">
+        <v>10</v>
+      </c>
+      <c r="P28" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -3804,8 +4050,14 @@
       <c r="B29">
         <v>4356</v>
       </c>
+      <c r="O29" t="s">
+        <v>10</v>
+      </c>
+      <c r="P29" t="s">
+        <v>10</v>
+      </c>
       <c r="Q29" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -3815,279 +4067,761 @@
       <c r="B30">
         <v>4199</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>10</v>
+      </c>
+      <c r="P30" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>10</v>
+      </c>
+      <c r="P31" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>10</v>
+      </c>
+      <c r="P32" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>10</v>
+      </c>
+      <c r="P33" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>10</v>
+      </c>
+      <c r="P34" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="O35" t="s">
+        <v>10</v>
+      </c>
+      <c r="P35" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="O36" t="s">
+        <v>10</v>
+      </c>
+      <c r="P36" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37">
         <v>3347</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O37" t="s">
+        <v>10</v>
+      </c>
+      <c r="P37" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="B38">
         <v>3746</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O38" t="s">
+        <v>10</v>
+      </c>
+      <c r="P38" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
       <c r="B39">
         <v>3588</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O39" t="s">
+        <v>10</v>
+      </c>
+      <c r="P39" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="B40">
         <v>3571</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O40" t="s">
+        <v>10</v>
+      </c>
+      <c r="P40" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5</v>
       </c>
       <c r="B41">
         <v>3805</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O41" t="s">
+        <v>10</v>
+      </c>
+      <c r="P41" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6</v>
       </c>
       <c r="B42">
         <v>3506</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O42" t="s">
+        <v>10</v>
+      </c>
+      <c r="P42" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>7</v>
       </c>
       <c r="B43">
         <v>3824</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O43" t="s">
+        <v>10</v>
+      </c>
+      <c r="P43" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>8</v>
       </c>
       <c r="B44">
         <v>3626</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O44" t="s">
+        <v>10</v>
+      </c>
+      <c r="P44" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
       <c r="B45">
         <v>3677</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O45" t="s">
+        <v>10</v>
+      </c>
+      <c r="P45" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10</v>
       </c>
       <c r="B46">
         <v>3782</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O46" t="s">
+        <v>10</v>
+      </c>
+      <c r="P46" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O47" t="s">
+        <v>10</v>
+      </c>
+      <c r="P47" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O48" t="s">
+        <v>10</v>
+      </c>
+      <c r="P48" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O49" t="s">
+        <v>10</v>
+      </c>
+      <c r="P49" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>10</v>
+      </c>
+      <c r="P50" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O51" t="s">
+        <v>10</v>
+      </c>
+      <c r="P51" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="O52" t="s">
+        <v>10</v>
+      </c>
+      <c r="P52" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="O53" t="s">
+        <v>10</v>
+      </c>
+      <c r="P53" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
       <c r="B54">
         <v>1353</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="O54" t="s">
+        <v>10</v>
+      </c>
+      <c r="P54" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
       <c r="B55">
         <v>1352</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+      <c r="O55" t="s">
+        <v>10</v>
+      </c>
+      <c r="P55" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
       <c r="B56">
         <v>1391</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="O56" t="s">
+        <v>10</v>
+      </c>
+      <c r="P56" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4</v>
       </c>
       <c r="B57">
         <v>1384</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="O57" t="s">
+        <v>10</v>
+      </c>
+      <c r="P57" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5</v>
       </c>
       <c r="B58">
         <v>1388</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="O58" t="s">
+        <v>10</v>
+      </c>
+      <c r="P58" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>6</v>
       </c>
       <c r="B59">
         <v>1393</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="O59" t="s">
+        <v>10</v>
+      </c>
+      <c r="P59" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>7</v>
       </c>
       <c r="B60">
         <v>1394</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+      <c r="O60" t="s">
+        <v>10</v>
+      </c>
+      <c r="P60" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>8</v>
       </c>
       <c r="B61">
         <v>1396</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="O61" t="s">
+        <v>10</v>
+      </c>
+      <c r="P61" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>9</v>
       </c>
       <c r="B62">
         <v>1366</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="O62" t="s">
+        <v>10</v>
+      </c>
+      <c r="P62" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>10</v>
       </c>
       <c r="B63">
         <v>1384</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="O63" t="s">
+        <v>10</v>
+      </c>
+      <c r="P63" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+      <c r="O64" t="s">
+        <v>10</v>
+      </c>
+      <c r="P64" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+      <c r="O65" t="s">
+        <v>10</v>
+      </c>
+      <c r="P65" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="O66" t="s">
+        <v>10</v>
+      </c>
+      <c r="P66" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1</v>
       </c>
       <c r="B67">
         <v>348</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="O67" t="s">
+        <v>10</v>
+      </c>
+      <c r="P67" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2</v>
       </c>
       <c r="B68">
         <v>344</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O68" t="s">
+        <v>10</v>
+      </c>
+      <c r="P68" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3</v>
       </c>
       <c r="B69">
         <v>359</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O69" t="s">
+        <v>10</v>
+      </c>
+      <c r="P69" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4</v>
       </c>
       <c r="B70">
         <v>351</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O70" t="s">
+        <v>10</v>
+      </c>
+      <c r="P70" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>5</v>
       </c>
       <c r="B71">
         <v>353</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O71" t="s">
+        <v>10</v>
+      </c>
+      <c r="P71" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>6</v>
       </c>
       <c r="B72">
         <v>349</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O72" t="s">
+        <v>10</v>
+      </c>
+      <c r="P72" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>7</v>
       </c>
       <c r="B73">
         <v>350</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O73" t="s">
+        <v>10</v>
+      </c>
+      <c r="P73" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>8</v>
       </c>
       <c r="B74">
         <v>356</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O74" t="s">
+        <v>10</v>
+      </c>
+      <c r="P74" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>9</v>
       </c>
       <c r="B75">
         <v>353</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O75" t="s">
+        <v>10</v>
+      </c>
+      <c r="P75" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10</v>
       </c>
@@ -4095,97 +4829,521 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="G80" t="s">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>8</v>
+      </c>
+      <c r="J80" t="s">
+        <v>1</v>
+      </c>
+      <c r="K80" t="s">
+        <v>8</v>
+      </c>
+      <c r="M80" t="s">
+        <v>1</v>
+      </c>
+      <c r="N80" t="s">
+        <v>8</v>
+      </c>
+      <c r="P80" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>8</v>
+      </c>
+      <c r="S80" t="s">
+        <v>1</v>
+      </c>
+      <c r="T80" t="s">
+        <v>8</v>
+      </c>
+      <c r="V80" t="s">
+        <v>1</v>
+      </c>
+      <c r="W80" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1</v>
       </c>
       <c r="B81">
         <v>244</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>318</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>316</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>248</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="P81">
+        <v>1</v>
+      </c>
+      <c r="S81">
+        <v>1</v>
+      </c>
+      <c r="V81">
+        <v>1</v>
+      </c>
+      <c r="Y81">
+        <v>1</v>
+      </c>
+      <c r="AB81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2</v>
       </c>
       <c r="B82">
         <v>234</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>327</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="H82">
+        <v>338</v>
+      </c>
+      <c r="J82">
+        <v>2</v>
+      </c>
+      <c r="K82">
+        <v>248</v>
+      </c>
+      <c r="M82">
+        <v>2</v>
+      </c>
+      <c r="P82">
+        <v>2</v>
+      </c>
+      <c r="S82">
+        <v>2</v>
+      </c>
+      <c r="V82">
+        <v>2</v>
+      </c>
+      <c r="Y82">
+        <v>2</v>
+      </c>
+      <c r="AB82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>3</v>
       </c>
       <c r="B83">
         <v>241</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83">
+        <v>336</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+      <c r="H83">
+        <v>333</v>
+      </c>
+      <c r="J83">
+        <v>3</v>
+      </c>
+      <c r="K83">
+        <v>245</v>
+      </c>
+      <c r="M83">
+        <v>3</v>
+      </c>
+      <c r="P83">
+        <v>3</v>
+      </c>
+      <c r="S83">
+        <v>3</v>
+      </c>
+      <c r="V83">
+        <v>3</v>
+      </c>
+      <c r="Y83">
+        <v>3</v>
+      </c>
+      <c r="AB83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
       <c r="B84">
         <v>243</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>4</v>
+      </c>
+      <c r="E84">
+        <v>333</v>
+      </c>
+      <c r="G84">
+        <v>4</v>
+      </c>
+      <c r="H84">
+        <v>332</v>
+      </c>
+      <c r="J84">
+        <v>4</v>
+      </c>
+      <c r="K84">
+        <v>247</v>
+      </c>
+      <c r="M84">
+        <v>4</v>
+      </c>
+      <c r="P84">
+        <v>4</v>
+      </c>
+      <c r="S84">
+        <v>4</v>
+      </c>
+      <c r="V84">
+        <v>4</v>
+      </c>
+      <c r="Y84">
+        <v>4</v>
+      </c>
+      <c r="AB84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>5</v>
       </c>
       <c r="B85">
         <v>242</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>5</v>
+      </c>
+      <c r="E85">
+        <v>337</v>
+      </c>
+      <c r="G85">
+        <v>5</v>
+      </c>
+      <c r="H85">
+        <v>330</v>
+      </c>
+      <c r="J85">
+        <v>5</v>
+      </c>
+      <c r="K85">
+        <v>250</v>
+      </c>
+      <c r="M85">
+        <v>5</v>
+      </c>
+      <c r="P85">
+        <v>5</v>
+      </c>
+      <c r="S85">
+        <v>5</v>
+      </c>
+      <c r="V85">
+        <v>5</v>
+      </c>
+      <c r="Y85">
+        <v>5</v>
+      </c>
+      <c r="AB85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>6</v>
       </c>
       <c r="B86">
         <v>241</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>6</v>
+      </c>
+      <c r="E86">
+        <v>334</v>
+      </c>
+      <c r="G86">
+        <v>6</v>
+      </c>
+      <c r="H86">
+        <v>317</v>
+      </c>
+      <c r="J86">
+        <v>6</v>
+      </c>
+      <c r="K86">
+        <v>246</v>
+      </c>
+      <c r="M86">
+        <v>6</v>
+      </c>
+      <c r="P86">
+        <v>6</v>
+      </c>
+      <c r="S86">
+        <v>6</v>
+      </c>
+      <c r="V86">
+        <v>6</v>
+      </c>
+      <c r="Y86">
+        <v>6</v>
+      </c>
+      <c r="AB86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>7</v>
       </c>
       <c r="B87">
         <v>243</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>7</v>
+      </c>
+      <c r="E87">
+        <v>335</v>
+      </c>
+      <c r="G87">
+        <v>7</v>
+      </c>
+      <c r="H87">
+        <v>302</v>
+      </c>
+      <c r="J87">
+        <v>7</v>
+      </c>
+      <c r="K87">
+        <v>254</v>
+      </c>
+      <c r="M87">
+        <v>7</v>
+      </c>
+      <c r="P87">
+        <v>7</v>
+      </c>
+      <c r="S87">
+        <v>7</v>
+      </c>
+      <c r="V87">
+        <v>7</v>
+      </c>
+      <c r="Y87">
+        <v>7</v>
+      </c>
+      <c r="AB87">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8</v>
       </c>
       <c r="B88">
         <v>245</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>8</v>
+      </c>
+      <c r="E88">
+        <v>338</v>
+      </c>
+      <c r="G88">
+        <v>8</v>
+      </c>
+      <c r="H88">
+        <v>295</v>
+      </c>
+      <c r="J88">
+        <v>8</v>
+      </c>
+      <c r="K88">
+        <v>250</v>
+      </c>
+      <c r="M88">
+        <v>8</v>
+      </c>
+      <c r="P88">
+        <v>8</v>
+      </c>
+      <c r="S88">
+        <v>8</v>
+      </c>
+      <c r="V88">
+        <v>8</v>
+      </c>
+      <c r="Y88">
+        <v>8</v>
+      </c>
+      <c r="AB88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>9</v>
       </c>
       <c r="B89">
         <v>243</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>9</v>
+      </c>
+      <c r="E89">
+        <v>335</v>
+      </c>
+      <c r="G89">
+        <v>9</v>
+      </c>
+      <c r="H89">
+        <v>324</v>
+      </c>
+      <c r="J89">
+        <v>9</v>
+      </c>
+      <c r="K89">
+        <v>247</v>
+      </c>
+      <c r="M89">
+        <v>9</v>
+      </c>
+      <c r="P89">
+        <v>9</v>
+      </c>
+      <c r="S89">
+        <v>9</v>
+      </c>
+      <c r="V89">
+        <v>9</v>
+      </c>
+      <c r="Y89">
+        <v>9</v>
+      </c>
+      <c r="AB89">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>10</v>
       </c>
       <c r="B90">
         <v>244</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+      <c r="E90">
+        <v>336</v>
+      </c>
+      <c r="G90">
+        <v>10</v>
+      </c>
+      <c r="H90">
+        <v>311</v>
+      </c>
+      <c r="J90">
+        <v>10</v>
+      </c>
+      <c r="K90">
+        <v>252</v>
+      </c>
+      <c r="M90">
+        <v>10</v>
+      </c>
+      <c r="P90">
+        <v>10</v>
+      </c>
+      <c r="S90">
+        <v>10</v>
+      </c>
+      <c r="V90">
+        <v>10</v>
+      </c>
+      <c r="Y90">
+        <v>10</v>
+      </c>
+      <c r="AB90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="K91">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="K92">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>